<commit_message>
Committing loads of changes
</commit_message>
<xml_diff>
--- a/Semester8/lab/exp7/exp7data.xlsx
+++ b/Semester8/lab/exp7/exp7data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>Init (cm)</t>
   </si>
@@ -41,13 +41,27 @@
   <si>
     <t>Diff</t>
   </si>
+  <si>
+    <t>Container Radius (cm)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -63,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,12 +85,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -199,48 +232,59 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$1:$E$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+            <c:strRef>
+              <c:f>Sheet1!$E$2:$E$18</c:f>
+              <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>8.92</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>Diameter (cm)</c:v>
+                </c:pt>
                 <c:pt idx="4">
                   <c:v>6.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Diameter (cm)</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8.15</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diameter (cm)</c:v>
+                </c:pt>
                 <c:pt idx="12">
                   <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Diameter (cm)</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>10.7</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$1:$F$17</c:f>
+              <c:f>Sheet1!$G$2:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.00">
                   <c:v>2.4666666666666663</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="4" formatCode="0.00">
                   <c:v>1.8999999999999997</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="8" formatCode="0.00">
                   <c:v>2.35</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="12" formatCode="0.00">
                   <c:v>1.4666666666666668</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="16" formatCode="0.00">
                   <c:v>3.0500000000000003</c:v>
                 </c:pt>
               </c:numCache>
@@ -256,11 +300,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="439401968"/>
-        <c:axId val="439409584"/>
+        <c:axId val="-1049120144"/>
+        <c:axId val="-1049119600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="439401968"/>
+        <c:axId val="-1049120144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -317,12 +361,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439409584"/>
+        <c:crossAx val="-1049119600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="439409584"/>
+        <c:axId val="-1049119600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -342,7 +386,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -379,7 +423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439401968"/>
+        <c:crossAx val="-1049120144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -990,13 +1034,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1282,299 +1326,354 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1">
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E2">
         <v>8.92</v>
       </c>
-      <c r="F1">
-        <f>AVERAGE(C2:C4)</f>
+      <c r="F2">
+        <f>E2/2</f>
+        <v>4.46</v>
+      </c>
+      <c r="G2" s="1">
+        <f>AVERAGE(C3:C5)</f>
         <v>2.4666666666666663</v>
       </c>
-      <c r="G1">
-        <f>_xlfn.STDEV.S(C2:C4)</f>
+      <c r="H2" s="2">
+        <f>_xlfn.STDEV.S(C3:C5)</f>
         <v>7.6376261582597263E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="4">
         <v>3.5</v>
       </c>
-      <c r="C2">
-        <f>B2-A2</f>
+      <c r="C3" s="4">
+        <f>B3-A3</f>
         <v>2.4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="4">
         <v>3.45</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C4" si="0">B3-A3</f>
+      <c r="C4" s="4">
+        <f t="shared" ref="C4:C5" si="0">B4-A4</f>
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="4">
         <v>3.65</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="4">
         <f t="shared" si="0"/>
         <v>2.5499999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+      <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E5">
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6">
         <v>6.38</v>
       </c>
-      <c r="F5">
-        <f>AVERAGE(C6:C8)</f>
+      <c r="F6">
+        <f>E6/2</f>
+        <v>3.19</v>
+      </c>
+      <c r="G6" s="1">
+        <f>AVERAGE(C7:C9)</f>
         <v>1.8999999999999997</v>
       </c>
-      <c r="G5">
-        <f>_xlfn.STDEV.S(C6:C8)</f>
+      <c r="H6" s="2">
+        <f>_xlfn.STDEV.S(C7:C9)</f>
         <v>4.9999999999999933E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>1.7</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="4">
         <v>3.65</v>
       </c>
-      <c r="C6">
-        <f>B6-A6</f>
+      <c r="C7" s="4">
+        <f>B7-A7</f>
         <v>1.95</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>1.65</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="4">
         <v>3.5</v>
       </c>
-      <c r="C7">
-        <f t="shared" ref="C7:C8" si="1">B7-A7</f>
+      <c r="C8" s="4">
+        <f t="shared" ref="C8:C9" si="1">B8-A8</f>
         <v>1.85</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>1.65</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="4">
         <v>3.55</v>
       </c>
-      <c r="C8">
+      <c r="C9" s="4">
         <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+      <c r="E9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9">
+      <c r="F9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10">
         <v>8.15</v>
       </c>
-      <c r="F9">
-        <f>AVERAGE(C10:C12)</f>
+      <c r="F10">
+        <f>E10/2</f>
+        <v>4.0750000000000002</v>
+      </c>
+      <c r="G10" s="1">
+        <f>AVERAGE(C11:C13)</f>
         <v>2.35</v>
       </c>
-      <c r="G9">
-        <f>_xlfn.STDEV.S(C10:C12)</f>
+      <c r="H10" s="2">
+        <f>_xlfn.STDEV.S(C11:C13)</f>
         <v>0.13228756555322957</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>1.5</v>
       </c>
-      <c r="B10">
+      <c r="B11" s="4">
         <v>3.7</v>
       </c>
-      <c r="C10">
-        <f>B10-A10</f>
+      <c r="C11" s="4">
+        <f>B11-A11</f>
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>1.55</v>
       </c>
-      <c r="B11">
+      <c r="B12" s="4">
         <v>4</v>
       </c>
-      <c r="C11">
-        <f t="shared" ref="C11:C12" si="2">B11-A11</f>
+      <c r="C12" s="4">
+        <f t="shared" ref="C12:C13" si="2">B12-A12</f>
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>1.55</v>
       </c>
-      <c r="B12">
+      <c r="B13" s="4">
         <v>3.95</v>
       </c>
-      <c r="C12">
+      <c r="C13" s="4">
         <f t="shared" si="2"/>
         <v>2.4000000000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+      <c r="E13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E13">
+      <c r="F13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14">
         <v>5.25</v>
       </c>
-      <c r="F13">
-        <f>AVERAGE(C14:C16)</f>
+      <c r="F14">
+        <f>E14/2</f>
+        <v>2.625</v>
+      </c>
+      <c r="G14" s="1">
+        <f>AVERAGE(C15:C17)</f>
         <v>1.4666666666666668</v>
       </c>
-      <c r="G13">
-        <f>_xlfn.STDEV.S(C14:C16)</f>
+      <c r="H14" s="2">
+        <f>_xlfn.STDEV.S(C15:C17)</f>
         <v>7.6376261582597374E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>1.45</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="4">
         <v>3</v>
       </c>
-      <c r="C14">
-        <f>B14-A14</f>
+      <c r="C15" s="4">
+        <f>B15-A15</f>
         <v>1.55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>1.4</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="4">
         <v>2.85</v>
       </c>
-      <c r="C15">
-        <f t="shared" ref="C15:C16" si="3">B15-A15</f>
+      <c r="C16" s="4">
+        <f t="shared" ref="C16:C17" si="3">B16-A16</f>
         <v>1.4500000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>1.4</v>
       </c>
-      <c r="B16">
+      <c r="B17" s="4">
         <v>2.8</v>
       </c>
-      <c r="C16">
+      <c r="C17" s="4">
         <f t="shared" si="3"/>
         <v>1.4</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+      <c r="E17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E17">
+      <c r="F17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E18">
         <v>10.7</v>
       </c>
-      <c r="F17">
-        <f>AVERAGE(C18:C20)</f>
+      <c r="F18">
+        <f>E18/2</f>
+        <v>5.35</v>
+      </c>
+      <c r="G18" s="1">
+        <f>AVERAGE(C19:C21)</f>
         <v>3.0500000000000003</v>
       </c>
-      <c r="G17">
-        <f>_xlfn.STDEV.S(C18:C20)</f>
+      <c r="H18" s="2">
+        <f>_xlfn.STDEV.S(C19:C21)</f>
         <v>0.18027756377319951</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>0</v>
       </c>
-      <c r="B18">
+      <c r="B19" s="4">
         <v>2.85</v>
       </c>
-      <c r="C18">
-        <f t="shared" ref="C18:C20" si="4">B18-A18</f>
+      <c r="C19" s="4">
+        <f t="shared" ref="C19:C21" si="4">B19-A19</f>
         <v>2.85</v>
       </c>
-      <c r="I18">
+      <c r="I19">
         <v>5.25</v>
       </c>
-      <c r="J18">
+      <c r="J19">
         <v>6.55</v>
       </c>
-      <c r="K18">
-        <f>J18-I18</f>
+      <c r="K19">
+        <f>J19-I19</f>
         <v>1.2999999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>0.3</v>
       </c>
-      <c r="B19">
+      <c r="B20" s="4">
         <v>3.4</v>
       </c>
-      <c r="C19">
+      <c r="C20" s="4">
         <f t="shared" si="4"/>
         <v>3.1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>0.25</v>
       </c>
-      <c r="B20">
+      <c r="B21" s="4">
         <v>3.45</v>
       </c>
-      <c r="C20">
+      <c r="C21" s="4">
         <f t="shared" si="4"/>
         <v>3.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>